<commit_message>
Updated the self evaluation sheet
</commit_message>
<xml_diff>
--- a/Decision Trees - ID3/IA_2324_GroupEvaluation_TP3_Group9.xlsx
+++ b/Decision Trees - ID3/IA_2324_GroupEvaluation_TP3_Group9.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1FD0597-DD0E-48CC-9A36-5BCB704C39E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D7ECF19-C2A4-46C3-B685-25C1B5AADA19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Student</t>
   </si>
@@ -47,13 +47,28 @@
   </si>
   <si>
     <t>% of participation in the project (sum of all students should be = 100%)</t>
+  </si>
+  <si>
+    <t>Responsible for implementing the data preprocessing mechanisms for the datasets utilized as well as to proper evaluate them and document their behaviour. In addition, he also recorded, edited and reviewed the video presentation.</t>
+  </si>
+  <si>
+    <t>Did not develop any kind of work</t>
+  </si>
+  <si>
+    <t>The Student did not engage on the project's development throughout the pratical classes nor on extra efforts apart from university. Moreover, he did not display any effort or commitment on working in the project.</t>
+  </si>
+  <si>
+    <t>~</t>
+  </si>
+  <si>
+    <t>Developed the ID3 Algorithm as well as a few data visualization functions to better visualize the behaviour of the model on each dataset. In addition, he also integrated the ID3 Algorithm inside the Connect Four game and analysed the result's obtained.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,6 +89,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -83,7 +106,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -106,11 +129,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -128,6 +190,19 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D3:G9"/>
+  <dimension ref="D3:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,7 +495,7 @@
     <col min="4" max="4" width="27.28515625" customWidth="1"/>
     <col min="5" max="5" width="32.7109375" customWidth="1"/>
     <col min="6" max="6" width="107.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41.28515625" customWidth="1"/>
+    <col min="7" max="7" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="4:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -447,29 +522,50 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="4:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="4:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="4:7" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="4:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="6">
+        <v>0</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="4:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="4"/>
+      <c r="E9" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="F13" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>